<commit_message>
Initial Commit: EaziRent Real Estate Escrow Protocol
</commit_message>
<xml_diff>
--- a/static/uploads/responses.xlsx
+++ b/static/uploads/responses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:W19"/>
+  <dimension ref="A3:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,6 +1204,123 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-02-12 15:44:47</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sometimes</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Never</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Once</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>I know exactly where to go</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Somewhat uncomfortable</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Disagree</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Sometimes</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Rarely</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Somewhat</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Rarely</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Rarely</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>I thought about it</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Disagree</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>A few times</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>A little</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Sometimes</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Very uncomfortable</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Disagree</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>Slightly confident</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>